<commit_message>
requirement / documentation change.
</commit_message>
<xml_diff>
--- a/documentation/models.xlsx
+++ b/documentation/models.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="31">
   <si>
     <t>EXP</t>
   </si>
@@ -45,9 +45,6 @@
     <t>USER</t>
   </si>
   <si>
-    <t>O_TASK</t>
-  </si>
-  <si>
     <t>tid</t>
   </si>
   <si>
@@ -106,13 +103,19 @@
   </si>
   <si>
     <t>public, friend, public</t>
+  </si>
+  <si>
+    <t>ouid</t>
+  </si>
+  <si>
+    <t>TASK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -166,8 +169,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -177,6 +205,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -273,7 +307,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -286,6 +320,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -316,8 +351,24 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -621,8 +672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,15 +685,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="12"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="13"/>
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -696,36 +747,38 @@
       <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A6" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="19"/>
+      <c r="A6" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="20"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="F7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="4"/>
+        <v>15</v>
+      </c>
+      <c r="G7" s="21" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
@@ -755,31 +808,31 @@
       <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A11" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="19"/>
+      <c r="A11" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="20"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>17</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" s="20" t="s">
-        <v>27</v>
+        <v>13</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>26</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="4"/>
@@ -790,7 +843,7 @@
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="4"/>
@@ -801,37 +854,37 @@
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="8"/>
     </row>
     <row r="16" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="15"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="16"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>26</v>
+        <v>13</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>25</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="4"/>
@@ -855,25 +908,25 @@
       <c r="G19" s="8"/>
     </row>
     <row r="21" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A21" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="15"/>
+      <c r="A21" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="16"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
@@ -899,22 +952,22 @@
       <c r="G24" s="8"/>
     </row>
     <row r="26" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A26" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="15"/>
+      <c r="A26" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="16"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -941,71 +994,71 @@
       <c r="G29" s="8"/>
     </row>
     <row r="31" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A31" s="13" t="s">
+      <c r="A31" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B31" s="24"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="25"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="B31" s="14"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="15"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+      <c r="B32" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="C32" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="F32" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G32" s="27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="28"/>
+      <c r="B33" s="22"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="22"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="29"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="30"/>
+      <c r="B34" s="31"/>
+      <c r="C34" s="31"/>
+      <c r="D34" s="31"/>
+      <c r="E34" s="31"/>
+      <c r="F34" s="31"/>
+      <c r="G34" s="32"/>
+    </row>
+    <row r="36" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A36" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C32" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E32" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F32" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="G32" s="21" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="5"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="4"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="6"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="8"/>
-    </row>
-    <row r="36" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A36" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="14"/>
-      <c r="G36" s="15"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="15"/>
+      <c r="G36" s="16"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
php&js set up for comment evetn
</commit_message>
<xml_diff>
--- a/documentation/models.xlsx
+++ b/documentation/models.xlsx
@@ -234,10 +234,6 @@
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
-    <t>me share task</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
     <t>myfollow share task</t>
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
@@ -271,6 +267,10 @@
   </si>
   <si>
     <t>[uid1]put comment on [uid2]'s [cid]</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>me PUBLISH task</t>
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
 </sst>
@@ -1363,7 +1363,7 @@
   <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B17"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -1413,7 +1413,7 @@
         <v>58</v>
       </c>
       <c r="C3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
@@ -1467,7 +1467,7 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C9" t="s">
         <v>53</v>
@@ -1486,7 +1486,7 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="C11" t="s">
         <v>54</v>
@@ -1497,7 +1497,7 @@
         <v>5.3333333333333304</v>
       </c>
       <c r="B12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -1505,7 +1505,7 @@
         <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C13" t="s">
         <v>55</v>
@@ -1516,7 +1516,7 @@
         <v>6.3333333333333304</v>
       </c>
       <c r="B14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1524,7 +1524,7 @@
         <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C15" t="s">
         <v>57</v>
@@ -1538,7 +1538,7 @@
         <v>7.3333333333333304</v>
       </c>
       <c r="B16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1546,7 +1546,7 @@
         <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C17" t="s">
         <v>56</v>
@@ -1557,7 +1557,7 @@
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>